<commit_message>
one code fixed in the print_out document, re-ran all analyses thereafter
</commit_message>
<xml_diff>
--- a/results/Tbl1.xlsx
+++ b/results/Tbl1.xlsx
@@ -139,6 +139,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -651,7 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -681,6 +684,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1004,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1090,22 +1094,22 @@
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="15">
         <v>0.95673076923076905</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="15">
         <v>0.88650525525525503</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="15">
         <v>0.91798565807186505</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="15">
         <v>0.95673076923076905</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="15">
         <v>0.89274279615795105</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="15">
         <v>0.92471970101441503</v>
       </c>
     </row>
@@ -1116,22 +1120,22 @@
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="15">
         <v>0.76923076923076905</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="15">
         <v>0.47264632420882402</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="15">
         <v>0.60559797197728205</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="15">
         <v>0.76923076923076905</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="15">
         <v>0.48132337246531498</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="15">
         <v>0.62520021356113198</v>
       </c>
     </row>
@@ -1142,22 +1146,22 @@
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="15">
         <v>1.3442841880341901E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="15">
         <v>7.2881686482155206E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="15">
         <v>4.6236687177894101E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="15">
         <v>1.3442841880341901E-2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="15">
         <v>7.1198025613660607E-2</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="15">
         <v>4.2335851575013399E-2</v>
       </c>
     </row>
@@ -1168,22 +1172,22 @@
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="15">
         <v>2.3647380793106701E-2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="15">
         <v>0.194587268820476</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="15">
         <v>0.147730391371655</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="15">
         <v>3.6809053304511098E-2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="15">
         <v>0.20152302138663</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="15">
         <v>0.147723506725531</v>
       </c>
     </row>
@@ -1192,12 +1196,12 @@
         <v>15</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -1206,22 +1210,22 @@
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="15">
         <v>0.98183760683760701</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="15">
         <v>0.91653997747747795</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="15">
         <v>0.94581132856994898</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="15">
         <v>0.98183760683760701</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="15">
         <v>0.92320000000000002</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="15">
         <v>0.952495329597011</v>
       </c>
     </row>
@@ -1232,22 +1236,22 @@
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="15">
         <v>0.83867521367521403</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="15">
         <v>0.55592623873873903</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="15">
         <v>0.682675779227503</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="15">
         <v>0.83867521367521403</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="15">
         <v>0.56640000000000001</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="15">
         <v>0.70242860955430997</v>
       </c>
     </row>
@@ -1258,22 +1262,22 @@
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="15">
         <v>7.9059829059829109E-3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="15">
         <v>2.7716315221471499E-2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="15">
         <v>1.8835821424873101E-2</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="15">
         <v>7.9059829059829109E-3</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="15">
         <v>2.4960053333333301E-2</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="15">
         <v>1.6439845209500901E-2</v>
       </c>
     </row>
@@ -1284,22 +1288,22 @@
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="15">
         <v>1.5621805866352799E-2</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="15">
         <v>4.07689852697906E-2</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="15">
         <v>3.3382413246185599E-2</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="15">
         <v>2.64789323896912E-2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="15">
         <v>5.2529342910345597E-2</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="15">
         <v>4.2465572253037598E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Decided to double check that new ratio coding was accurate throughout the workflow.
</commit_message>
<xml_diff>
--- a/results/Tbl1.xlsx
+++ b/results/Tbl1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\how_many_replicators\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\how_many_replicators\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942832BD-7D4F-4324-AC59-D4C7698A07EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tbl1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Team-Level</t>
   </si>
@@ -133,12 +134,18 @@
   </si>
   <si>
     <t>1-question (5 ordinal responses)</t>
+  </si>
+  <si>
+    <t>Team-Level Dichotomy</t>
+  </si>
+  <si>
+    <t>Trimmed Replication Results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -681,10 +688,10 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1005,34 +1012,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H13"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" style="5" customWidth="1"/>
-    <col min="3" max="8" width="6.90625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="21.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="5" customWidth="1"/>
+    <col min="3" max="8" width="6.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1057,8 +1067,17 @@
       <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1080,530 +1099,769 @@
       <c r="H3" s="4">
         <v>3746</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="2">
+        <v>39</v>
+      </c>
+      <c r="J3" s="2">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>0.95673076923076905</v>
       </c>
-      <c r="D5" s="15">
-        <v>0.88650525525525503</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0.91798565807186505</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="D5" s="14">
+        <v>0.89220917822838897</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.92445274959957302</v>
+      </c>
+      <c r="F5" s="14">
         <v>0.95673076923076905</v>
       </c>
-      <c r="G5" s="15">
-        <v>0.89274279615795105</v>
-      </c>
-      <c r="H5" s="15">
-        <v>0.92471970101441503</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="14">
+        <v>0.885971067221067</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.91769093363920995</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0.79487179487179505</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.65217391304347805</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0.71764705882352897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15">
-        <v>0.76923076923076905</v>
-      </c>
-      <c r="D6" s="15">
-        <v>0.47264632420882402</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.60559797197728205</v>
-      </c>
-      <c r="F6" s="15">
-        <v>0.76923076923076905</v>
-      </c>
-      <c r="G6" s="15">
-        <v>0.48132337246531498</v>
-      </c>
-      <c r="H6" s="15">
-        <v>0.62520021356113198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="14">
+        <v>0.77403846153846201</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.50053361792956197</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.63721302722904405</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.77403846153846201</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.49138296950797</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.61809060386646597</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="J6" s="14">
+        <v>6.5217391304347797E-2</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0.317647058823529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15">
-        <v>1.3442841880341901E-2</v>
-      </c>
-      <c r="D7" s="15">
-        <v>7.2881686482155206E-2</v>
-      </c>
-      <c r="E7" s="15">
-        <v>4.6236687177894101E-2</v>
-      </c>
-      <c r="F7" s="15">
-        <v>1.3442841880341901E-2</v>
-      </c>
-      <c r="G7" s="15">
-        <v>7.1198025613660607E-2</v>
-      </c>
-      <c r="H7" s="15">
-        <v>4.2335851575013399E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="14">
+        <v>1.37323717948718E-2</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.32175880469583801</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.16782781633742699</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1.37323717948718E-2</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0.31831531351062597</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0.18177813274149501</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1.37323717948718E-2</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.328146776416885</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0.18388604959031399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="15">
-        <v>2.3647380793106701E-2</v>
-      </c>
-      <c r="D8" s="15">
-        <v>0.194587268820476</v>
-      </c>
-      <c r="E8" s="15">
-        <v>0.147730391371655</v>
-      </c>
-      <c r="F8" s="15">
-        <v>3.6809053304511098E-2</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.20152302138663</v>
-      </c>
-      <c r="H8" s="15">
-        <v>0.147723506725531</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="14">
+        <v>3.8119834945668299E-2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1.3842537609227501</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.99135636527690896</v>
+      </c>
+      <c r="F8" s="14">
+        <v>2.4326562186167199E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1.36253296080041</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1.0188569403063601</v>
+      </c>
+      <c r="I8" s="14">
+        <v>2.4326562186167199E-2</v>
+      </c>
+      <c r="J8" s="14">
+        <v>1.3916273411259601</v>
+      </c>
+      <c r="K8" s="14">
+        <v>1.03081763185549</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15">
-        <v>0.98183760683760701</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.91653997747747795</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0.94581132856994898</v>
-      </c>
-      <c r="F10" s="15">
-        <v>0.98183760683760701</v>
-      </c>
-      <c r="G10" s="15">
-        <v>0.92320000000000002</v>
-      </c>
-      <c r="H10" s="15">
-        <v>0.952495329597011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="14">
+        <v>0.96283783783783805</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.91893424036281202</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.94096045197740097</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.96283783783783805</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.91336913836913802</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.93569038081233202</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.83783783783783805</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.68181818181818199</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0.75308641975308599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="15">
-        <v>0.83867521367521403</v>
-      </c>
-      <c r="D11" s="15">
-        <v>0.55592623873873903</v>
-      </c>
-      <c r="E11" s="15">
-        <v>0.682675779227503</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0.83867521367521403</v>
-      </c>
-      <c r="G11" s="15">
-        <v>0.56640000000000001</v>
-      </c>
-      <c r="H11" s="15">
-        <v>0.70242860955430997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="14">
+        <v>0.80011261261261302</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.52721088435374197</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.66412429378531102</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.80011261261261302</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0.51969738969738999</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0.64622620979328305</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0.64864864864864902</v>
+      </c>
+      <c r="J11" s="14">
+        <v>6.8181818181818205E-2</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="15">
-        <v>7.9059829059829109E-3</v>
-      </c>
-      <c r="D12" s="15">
-        <v>2.7716315221471499E-2</v>
-      </c>
-      <c r="E12" s="15">
-        <v>1.8835821424873101E-2</v>
-      </c>
-      <c r="F12" s="15">
-        <v>7.9059829059829109E-3</v>
-      </c>
-      <c r="G12" s="15">
-        <v>2.4960053333333301E-2</v>
-      </c>
-      <c r="H12" s="15">
-        <v>1.6439845209500901E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="14">
+        <v>1.2252252252252301E-2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.33205102040816298</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.171609604519774</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1.2252252252252301E-2</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.329368371448371</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.186279390835488</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1.2252252252252301E-2</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.33508242534492499</v>
+      </c>
+      <c r="K12" s="14">
+        <v>0.18761679072234599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="15">
-        <v>1.5621805866352799E-2</v>
-      </c>
-      <c r="D13" s="15">
-        <v>4.07689852697906E-2</v>
-      </c>
-      <c r="E13" s="15">
-        <v>3.3382413246185599E-2</v>
-      </c>
-      <c r="F13" s="15">
-        <v>2.64789323896912E-2</v>
-      </c>
-      <c r="G13" s="15">
-        <v>5.2529342910345597E-2</v>
-      </c>
-      <c r="H13" s="15">
-        <v>4.2465572253037598E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="14">
+        <v>3.6505812703207803E-2</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1.4256735700790999</v>
+      </c>
+      <c r="E13" s="14">
+        <v>1.0192068422578899</v>
+      </c>
+      <c r="F13" s="14">
+        <v>2.4083207071360101E-2</v>
+      </c>
+      <c r="G13" s="14">
+        <v>1.4074745708276699</v>
+      </c>
+      <c r="H13" s="14">
+        <v>1.04955085868721</v>
+      </c>
+      <c r="I13" s="14">
+        <v>2.4083207071360101E-2</v>
+      </c>
+      <c r="J13" s="14">
+        <v>1.42321840938998</v>
+      </c>
+      <c r="K13" s="14">
+        <v>1.0560198699954799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.98183760683760701</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.92320000000000002</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.952495329597011</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.98183760683760701</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0.91653997747747795</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0.94581132856994898</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0.87179487179487203</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.76086956521739102</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0.81176470588235305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.845619658119658</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0.58826666666666705</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.71684013877768904</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.845619658119658</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0.57728040540540504</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.69757041524282903</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0.64102564102564097</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.13043478260869601</v>
+      </c>
+      <c r="K16" s="14">
+        <v>0.36470588235294099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="14">
+        <v>7.8605769230769198E-3</v>
+      </c>
+      <c r="D17" s="14">
+        <v>2.7221333333333299E-2</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1.7548705631171599E-2</v>
+      </c>
+      <c r="F17" s="14">
+        <v>7.8605769230769198E-3</v>
+      </c>
+      <c r="G17" s="14">
+        <v>3.0794359984985E-2</v>
+      </c>
+      <c r="H17" s="14">
+        <v>2.0513698612405502E-2</v>
+      </c>
+      <c r="I17" s="14">
+        <v>7.8605769230769198E-3</v>
+      </c>
+      <c r="J17" s="14">
+        <v>2.8124911868390098E-2</v>
+      </c>
+      <c r="K17" s="14">
+        <v>1.8827158187599401E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2.5993530118180699E-2</v>
+      </c>
+      <c r="D18" s="14">
+        <v>6.4056126780794698E-2</v>
+      </c>
+      <c r="E18" s="14">
+        <v>4.98386876241304E-2</v>
+      </c>
+      <c r="F18" s="14">
+        <v>1.53796164219028E-2</v>
+      </c>
+      <c r="G18" s="14">
+        <v>4.9848426574547598E-2</v>
+      </c>
+      <c r="H18" s="14">
+        <v>3.99263999504283E-2</v>
+      </c>
+      <c r="I18" s="14">
+        <v>1.53796164219028E-2</v>
+      </c>
+      <c r="J18" s="14">
+        <v>4.9106682545531001E-2</v>
+      </c>
+      <c r="K18" s="14">
+        <v>3.8756137699645601E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.63043478260869601</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.64705882352941202</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.487179487179487</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.49411764705882399</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3">
-        <v>-3.6631897039636402E-2</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.131830399452842</v>
-      </c>
-      <c r="E17" s="3">
-        <v>5.4535934003352202E-2</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="3">
-        <v>1.7859429892541301</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1.5392377445784</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1.6490251904106299</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2.1025641025641</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2.2391304347826102</v>
-      </c>
-      <c r="E19" s="3">
-        <v>2.1764705882352899</v>
-      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="C20" s="3">
-        <v>0.78789766216551504</v>
+        <v>0.66666666666666696</v>
       </c>
       <c r="D20" s="3">
-        <v>0.765500057586053</v>
+        <v>0.63043478260869601</v>
       </c>
       <c r="E20" s="3">
-        <v>0.77423496169468098</v>
+        <v>0.64705882352941202</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3">
-        <v>-8.84615384615383E-2</v>
+        <v>0.487179487179487</v>
       </c>
       <c r="D21" s="3">
-        <v>1.5217391304348E-2</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="3">
-        <v>-3.2352941176470397E-2</v>
+        <v>0.49411764705882399</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="6"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="C22" s="3">
-        <v>0.64261611058784096</v>
+        <v>-3.6631897039636402E-2</v>
       </c>
       <c r="D22" s="3">
-        <v>0.86028868315088802</v>
+        <v>0.131830399452842</v>
       </c>
       <c r="E22" s="3">
-        <v>0.76550270917816099</v>
+        <v>5.4535934003352202E-2</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>26</v>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="C23" s="3">
+        <v>1.7859429892541301</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.5392377445784</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1.6490251904106299</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3">
-        <v>0.230769230769231</v>
+        <v>2.1025641025641</v>
       </c>
       <c r="D24" s="3">
-        <v>0.3125</v>
+        <v>2.2391304347826102</v>
       </c>
       <c r="E24" s="3">
-        <v>0.28235294117647097</v>
+        <v>2.1764705882352899</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>28</v>
-      </c>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="6"/>
       <c r="C25" s="3">
-        <v>0.15384615384615399</v>
+        <v>0.78789766216551504</v>
       </c>
       <c r="D25" s="3">
-        <v>0.70833333333333304</v>
+        <v>0.765500057586053</v>
       </c>
       <c r="E25" s="3">
-        <v>0.47058823529411797</v>
+        <v>0.77423496169468098</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3">
-        <v>0.20512820512820501</v>
+        <v>-8.84615384615383E-2</v>
       </c>
       <c r="D26" s="3">
-        <v>0.20833333333333301</v>
+        <v>1.5217391304348E-2</v>
       </c>
       <c r="E26" s="3">
-        <v>0.21176470588235299</v>
+        <v>-3.2352941176470397E-2</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>28</v>
-      </c>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="6"/>
       <c r="C27" s="3">
-        <v>2.5641025641025599E-2</v>
+        <v>0.64261611058784096</v>
       </c>
       <c r="D27" s="3">
-        <v>6.25E-2</v>
+        <v>0.86028868315088802</v>
       </c>
       <c r="E27" s="3">
-        <v>4.7058823529411799E-2</v>
+        <v>0.76550270917816099</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E28" s="3">
-        <v>3.5294117647058802E-2</v>
-      </c>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.230769230769231</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.28235294117647097</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.15384615384615399</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.47058823529411797</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.20512820512820501</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.21176470588235299</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2.5641025641025599E-2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>4.7058823529411799E-2</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>3.5294117647058802E-2</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C34" s="13">
         <v>0</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D34" s="13">
         <v>6.25E-2</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E34" s="13">
         <v>3.5294117647058802E-2</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>